<commit_message>
Cleaned & formatted census tract added
</commit_message>
<xml_diff>
--- a/output_state_district_tract_map.xlsx
+++ b/output_state_district_tract_map.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>tract (or part)</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>CensusTract</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -489,6 +494,11 @@
           <t>000107</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -519,6 +529,11 @@
           <t>000109</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1.09 </t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -549,6 +564,11 @@
           <t>000115</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1.15</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -579,6 +599,11 @@
           <t>000118</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1.18</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -609,6 +634,11 @@
           <t>000120</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -639,6 +669,11 @@
           <t>000121</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1.21</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -669,6 +704,11 @@
           <t>000122</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1.22</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -699,6 +739,11 @@
           <t>000123</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1.23</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -729,6 +774,11 @@
           <t>000125</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -759,6 +809,11 @@
           <t>000126</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1.26</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -789,6 +844,11 @@
           <t>000127</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1.27</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -819,6 +879,11 @@
           <t>000128</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1.28 </t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -849,6 +914,11 @@
           <t>000129</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1.29</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -879,6 +949,11 @@
           <t>000130</t>
         </is>
       </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1.30</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -909,6 +984,11 @@
           <t>000131</t>
         </is>
       </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1.31</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -939,6 +1019,11 @@
           <t>000132</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1.32</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -969,6 +1054,11 @@
           <t>000134</t>
         </is>
       </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1.34</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -999,6 +1089,11 @@
           <t>000140</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1.40</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1029,6 +1124,11 @@
           <t>000141</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1.41</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1059,6 +1159,11 @@
           <t>000142</t>
         </is>
       </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1.42</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1089,6 +1194,11 @@
           <t>000143</t>
         </is>
       </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>1.43</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1119,6 +1229,11 @@
           <t>000144</t>
         </is>
       </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1149,6 +1264,11 @@
           <t>000145</t>
         </is>
       </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1.45</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1179,6 +1299,11 @@
           <t>000146</t>
         </is>
       </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1.46</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1209,6 +1334,11 @@
           <t>001204</t>
         </is>
       </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12.04 </t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1239,6 +1369,11 @@
           <t>003801</t>
         </is>
       </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">38.01 </t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1269,6 +1404,11 @@
           <t>003803</t>
         </is>
       </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>38.03</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1299,6 +1439,11 @@
           <t>003804</t>
         </is>
       </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>38.04</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1327,6 +1472,11 @@
       <c r="F30" t="inlineStr">
         <is>
           <t>990000</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">9900 </t>
         </is>
       </c>
     </row>

</xml_diff>